<commit_message>
Add JavaFX charts in Admin-Dashboard
</commit_message>
<xml_diff>
--- a/Assets/Docs/READ ME.xlsx
+++ b/Assets/Docs/READ ME.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Quantum Blaze\Projects\Research Project\POS Systems\POS_Java_01\Assets\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DB58EE-7BCD-4BFE-9BD7-E51F8EB04E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2DB2F2-FE86-4420-95F8-145B8F4331DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>employee username &amp; password manage කරන්න access තියෙන්නෙ owner කෙනෙක්ට විතරයි</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Traning veerification PIN number එක change කරන්න ඕන. Wrong PIN number එකක් enter කරන එක check කරන්න ඕන.</t>
   </si>
 </sst>
 </file>
@@ -372,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE43E60-A5DD-45A4-B6BB-129D0014AAFB}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,6 +414,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>